<commit_message>
updated files with corrected EX2303 sample names
</commit_message>
<xml_diff>
--- a/code/metadata-merge-20250723/input/Okeanos_Explorer_Sample_Track_Clement_LRT.xlsx
+++ b/code/metadata-merge-20250723/input/Okeanos_Explorer_Sample_Track_Clement_LRT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/T7A/Google Drive/NOAA/okex/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D737DC-3199-2F4C-976F-37452755CCF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC806C1C-005E-EA48-B023-CE1912BE28AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="28300" activeTab="2" xr2:uid="{0C776A5B-5EA3-A743-8078-B794F90EEA72}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{0C776A5B-5EA3-A743-8078-B794F90EEA72}"/>
   </bookViews>
   <sheets>
     <sheet name="Okeanos_Explorer_Sample_Track" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6565" uniqueCount="2422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6565" uniqueCount="2434">
   <si>
     <t>Data_type</t>
   </si>
@@ -7503,6 +7503,42 @@
   </si>
   <si>
     <t>Changes from Clement's file:</t>
+  </si>
+  <si>
+    <t>EX2303_CTD002_B01</t>
+  </si>
+  <si>
+    <t>EX2303_CTD002_B02</t>
+  </si>
+  <si>
+    <t>EX2303_CTD002_B03</t>
+  </si>
+  <si>
+    <t>EX2303_CTD002_B04</t>
+  </si>
+  <si>
+    <t>EX2303_CTD002_B05</t>
+  </si>
+  <si>
+    <t>EX2303_CTD002_B06</t>
+  </si>
+  <si>
+    <t>EX2303_CTD002_B07</t>
+  </si>
+  <si>
+    <t>EX2303_CTD002_B08</t>
+  </si>
+  <si>
+    <t>EX2303_CTD002_B09</t>
+  </si>
+  <si>
+    <t>EX2303_CTD002_B10</t>
+  </si>
+  <si>
+    <t>EX2303_CTD002_B11</t>
+  </si>
+  <si>
+    <t>EX2303_CTD002_B12</t>
   </si>
 </sst>
 </file>
@@ -8440,9 +8476,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I734"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A283" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G303" sqref="G303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12311,7 +12347,7 @@
         <v>1568</v>
       </c>
       <c r="I133" t="s">
-        <v>1829</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.2">
@@ -12340,7 +12376,7 @@
         <v>1569</v>
       </c>
       <c r="I134" t="s">
-        <v>1830</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
@@ -17121,11 +17157,11 @@
       <c r="G299" t="s">
         <v>1805</v>
       </c>
-      <c r="H299" t="s">
-        <v>1805</v>
-      </c>
-      <c r="I299" t="s">
-        <v>1805</v>
+      <c r="H299" s="4" t="s">
+        <v>2422</v>
+      </c>
+      <c r="I299" s="4" t="s">
+        <v>2422</v>
       </c>
     </row>
     <row r="300" spans="1:9" x14ac:dyDescent="0.2">
@@ -17150,11 +17186,11 @@
       <c r="G300" t="s">
         <v>1806</v>
       </c>
-      <c r="H300" t="s">
-        <v>1806</v>
-      </c>
-      <c r="I300" t="s">
-        <v>1806</v>
+      <c r="H300" s="4" t="s">
+        <v>2423</v>
+      </c>
+      <c r="I300" s="4" t="s">
+        <v>2423</v>
       </c>
     </row>
     <row r="301" spans="1:9" x14ac:dyDescent="0.2">
@@ -17179,11 +17215,11 @@
       <c r="G301" t="s">
         <v>1807</v>
       </c>
-      <c r="H301" t="s">
-        <v>1807</v>
-      </c>
-      <c r="I301" t="s">
-        <v>1807</v>
+      <c r="H301" s="4" t="s">
+        <v>2424</v>
+      </c>
+      <c r="I301" s="4" t="s">
+        <v>2424</v>
       </c>
     </row>
     <row r="302" spans="1:9" x14ac:dyDescent="0.2">
@@ -17208,11 +17244,11 @@
       <c r="G302" t="s">
         <v>1808</v>
       </c>
-      <c r="H302" t="s">
-        <v>1808</v>
-      </c>
-      <c r="I302" t="s">
-        <v>1808</v>
+      <c r="H302" s="4" t="s">
+        <v>2425</v>
+      </c>
+      <c r="I302" s="4" t="s">
+        <v>2425</v>
       </c>
     </row>
     <row r="303" spans="1:9" x14ac:dyDescent="0.2">
@@ -17237,11 +17273,11 @@
       <c r="G303" t="s">
         <v>1809</v>
       </c>
-      <c r="H303" t="s">
-        <v>1809</v>
-      </c>
-      <c r="I303" t="s">
-        <v>1809</v>
+      <c r="H303" s="4" t="s">
+        <v>2426</v>
+      </c>
+      <c r="I303" s="4" t="s">
+        <v>2426</v>
       </c>
     </row>
     <row r="304" spans="1:9" x14ac:dyDescent="0.2">
@@ -17266,11 +17302,11 @@
       <c r="G304" t="s">
         <v>1810</v>
       </c>
-      <c r="H304" t="s">
-        <v>1810</v>
-      </c>
-      <c r="I304" t="s">
-        <v>1810</v>
+      <c r="H304" s="4" t="s">
+        <v>2427</v>
+      </c>
+      <c r="I304" s="4" t="s">
+        <v>2427</v>
       </c>
     </row>
     <row r="305" spans="1:9" x14ac:dyDescent="0.2">
@@ -17295,11 +17331,11 @@
       <c r="G305" t="s">
         <v>1811</v>
       </c>
-      <c r="H305" t="s">
-        <v>1811</v>
-      </c>
-      <c r="I305" t="s">
-        <v>1811</v>
+      <c r="H305" s="4" t="s">
+        <v>2428</v>
+      </c>
+      <c r="I305" s="4" t="s">
+        <v>2428</v>
       </c>
     </row>
     <row r="306" spans="1:9" x14ac:dyDescent="0.2">
@@ -17324,11 +17360,11 @@
       <c r="G306" t="s">
         <v>1812</v>
       </c>
-      <c r="H306" t="s">
-        <v>1812</v>
-      </c>
-      <c r="I306" t="s">
-        <v>1812</v>
+      <c r="H306" s="4" t="s">
+        <v>2429</v>
+      </c>
+      <c r="I306" s="4" t="s">
+        <v>2429</v>
       </c>
     </row>
     <row r="307" spans="1:9" x14ac:dyDescent="0.2">
@@ -17353,11 +17389,11 @@
       <c r="G307" t="s">
         <v>1813</v>
       </c>
-      <c r="H307" t="s">
-        <v>1813</v>
-      </c>
-      <c r="I307" t="s">
-        <v>1813</v>
+      <c r="H307" s="4" t="s">
+        <v>2430</v>
+      </c>
+      <c r="I307" s="4" t="s">
+        <v>2430</v>
       </c>
     </row>
     <row r="308" spans="1:9" x14ac:dyDescent="0.2">
@@ -17382,11 +17418,11 @@
       <c r="G308" t="s">
         <v>1814</v>
       </c>
-      <c r="H308" t="s">
-        <v>1814</v>
-      </c>
-      <c r="I308" t="s">
-        <v>1814</v>
+      <c r="H308" s="4" t="s">
+        <v>2431</v>
+      </c>
+      <c r="I308" s="4" t="s">
+        <v>2431</v>
       </c>
     </row>
     <row r="309" spans="1:9" x14ac:dyDescent="0.2">
@@ -17411,11 +17447,11 @@
       <c r="G309" t="s">
         <v>1815</v>
       </c>
-      <c r="H309" t="s">
-        <v>1815</v>
-      </c>
-      <c r="I309" t="s">
-        <v>1815</v>
+      <c r="H309" s="4" t="s">
+        <v>2432</v>
+      </c>
+      <c r="I309" s="4" t="s">
+        <v>2432</v>
       </c>
     </row>
     <row r="310" spans="1:9" x14ac:dyDescent="0.2">
@@ -17440,11 +17476,11 @@
       <c r="G310" t="s">
         <v>1816</v>
       </c>
-      <c r="H310" t="s">
-        <v>1816</v>
-      </c>
-      <c r="I310" t="s">
-        <v>1816</v>
+      <c r="H310" s="4" t="s">
+        <v>2433</v>
+      </c>
+      <c r="I310" s="4" t="s">
+        <v>2433</v>
       </c>
     </row>
     <row r="311" spans="1:9" x14ac:dyDescent="0.2">
@@ -21098,7 +21134,7 @@
         <v>1568</v>
       </c>
       <c r="I436" t="s">
-        <v>1829</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="437" spans="1:9" x14ac:dyDescent="0.2">
@@ -21127,7 +21163,7 @@
         <v>1569</v>
       </c>
       <c r="I437" t="s">
-        <v>1830</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="438" spans="1:9" x14ac:dyDescent="0.2">
@@ -29817,7 +29853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FE0237C-4263-0140-B1F2-9707CB0320AD}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>